<commit_message>
api Modified by id
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D107"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,9 +456,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
+      <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
           <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%AB%D9%84%D8%A7%D8%AB%D9%8A%D8%A9_(%D9%86%D8%AC%D9%8A%D8%A8_%D9%85%D8%AD%D9%81%D9%88%D8%B8)</t>
@@ -476,9 +474,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
           <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%A8%D8%AD%D8%AB_%D8%B9%D9%86_%D9%88%D9%84%D9%8A%D8%AF_%D9%85%D8%B3%D8%B9%D9%88%D8%AF_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
@@ -497,16 +493,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B4%D8%B1%D9%81_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%AD%D8%B1%D8%A8_%D9%81%D9%8A_%D8%A8%D8%B1_%D9%85%D8%B5%D8%B1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B5%D9%86%D8%B9_%D8%A7%D9%84%D9%84%D9%87_%D8%A5%D8%A8%D8%B1%D8%A7%D9%87%D9%8A%D9%85</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%8A%D9%88%D8%B3%D9%81_%D8%A7%D9%84%D9%82%D8%B9%D9%8A%D8%AF</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -517,36 +513,36 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%AD%D8%B1%D8%A8_%D9%81%D9%8A_%D8%A8%D8%B1_%D9%85%D8%B5%D8%B1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B1%D8%AC%D8%A7%D9%84_%D9%81%D9%8A_%D8%A7%D9%84%D8%B4%D9%85%D8%B3_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%8A%D9%88%D8%B3%D9%81_%D8%A7%D9%84%D9%82%D8%B9%D9%8A%D8%AF</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%BA%D8%B3%D8%A7%D9%86_%D9%83%D9%86%D9%81%D8%A7%D9%86%D9%8A</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/مصر</t>
+          <t>https://ar.wikipedia.org/wiki/فلسطين</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B1%D8%AC%D8%A7%D9%84_%D9%81%D9%8A_%D8%A7%D9%84%D8%B4%D9%85%D8%B3_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%88%D9%82%D8%A7%D8%A6%D8%B9_%D8%A7%D9%84%D8%BA%D8%B1%D9%8A%D8%A8%D8%A9_%D9%81%D9%8A_%D8%A7%D8%AE%D8%AA%D9%81%D8%A7%D8%A1_%D8%B3%D8%B9%D9%8A%D8%AF_%D8%A3%D8%A8%D9%8A_%D8%A7%D9%84%D9%86%D8%AD%D8%B3_%D8%A7%D9%84%D9%85%D8%AA%D8%B4%D8%A7%D8%A6%D9%84</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%BA%D8%B3%D8%A7%D9%86_%D9%83%D9%86%D9%81%D8%A7%D9%86%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A5%D9%85%D9%8A%D9%84_%D8%AD%D8%A8%D9%8A%D8%A8%D9%8A</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -557,136 +553,136 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%88%D9%82%D8%A7%D8%A6%D8%B9_%D8%A7%D9%84%D8%BA%D8%B1%D9%8A%D8%A8%D8%A9_%D9%81%D9%8A_%D8%A7%D8%AE%D8%AA%D9%81%D8%A7%D8%A1_%D8%B3%D8%B9%D9%8A%D8%AF_%D8%A3%D8%A8%D9%8A_%D8%A7%D9%84%D9%86%D8%AD%D8%B3_%D8%A7%D9%84%D9%85%D8%AA%D8%B4%D8%A7%D8%A6%D9%84</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B2%D9%85%D9%86_%D8%A7%D9%84%D9%85%D9%88%D8%AD%D8%B4</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A5%D9%85%D9%8A%D9%84_%D8%AD%D8%A8%D9%8A%D8%A8%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AD%D9%8A%D8%AF%D8%B1_%D8%AD%D9%8A%D8%AF%D8%B1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/فلسطين</t>
+          <t>https://ar.wikipedia.org/wiki/سوريا</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B2%D9%85%D9%86_%D8%A7%D9%84%D9%85%D9%88%D8%AD%D8%B4</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B1%D8%A7%D9%85%D8%A9_%D9%88%D8%A7%D9%84%D8%AA%D9%86%D9%8A%D9%86</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AD%D9%8A%D8%AF%D8%B1_%D8%AD%D9%8A%D8%AF%D8%B1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A5%D8%AF%D9%88%D8%A7%D8%B1_%D8%AE%D8%B1%D8%A7%D8%B7</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/سوريا</t>
+          <t>https://ar.wikipedia.org/wiki/مصر</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B1%D8%A7%D9%85%D8%A9_%D9%88%D8%A7%D9%84%D8%AA%D9%86%D9%8A%D9%86</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AD%D8%AF%D8%AB_%D8%A3%D8%A8%D9%88_%D9%87%D8%B1%D9%8A%D8%B1%D8%A9_%D9%82%D8%A7%D9%84</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A5%D8%AF%D9%88%D8%A7%D8%B1_%D8%AE%D8%B1%D8%A7%D8%B7</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D9%88%D8%AF_%D8%A7%D9%84%D9%85%D8%B3%D8%B9%D8%AF%D9%8A</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/مصر</t>
+          <t>https://ar.wikipedia.org/wiki/تونس</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AD%D8%AF%D8%AB_%D8%A3%D8%A8%D9%88_%D9%87%D8%B1%D9%8A%D8%B1%D8%A9_%D9%82%D8%A7%D9%84</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%83%D9%88%D8%A7%D8%A8%D9%8A%D8%B3_%D8%A8%D9%8A%D8%B1%D9%88%D8%AA</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D9%88%D8%AF_%D8%A7%D9%84%D9%85%D8%B3%D8%B9%D8%AF%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%BA%D8%A7%D8%AF%D8%A9_%D8%A7%D9%84%D8%B3%D9%85%D8%A7%D9%86</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/تونس</t>
+          <t>https://ar.wikipedia.org/wiki/سوريا</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%83%D9%88%D8%A7%D8%A8%D9%8A%D8%B3_%D8%A8%D9%8A%D8%B1%D9%88%D8%AA</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%85%D8%AC%D9%88%D8%B3_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%BA%D8%A7%D8%AF%D8%A9_%D8%A7%D9%84%D8%B3%D9%85%D8%A7%D9%86</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A5%D8%A8%D8%B1%D8%A7%D9%87%D9%8A%D9%85_%D8%A7%D9%84%D9%83%D9%88%D9%86%D9%8A</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/سوريا</t>
+          <t>https://ar.wikipedia.org/wiki/ليبيا</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%85%D8%AC%D9%88%D8%B3_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%88%D8%B4%D9%85_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A5%D8%A8%D8%B1%D8%A7%D9%87%D9%8A%D9%85_%D8%A7%D9%84%D9%83%D9%88%D9%86%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D8%B1%D8%AD%D9%85%D9%86_%D9%85%D8%AC%D9%8A%D8%AF_%D8%A7%D9%84%D8%B1%D8%A8%D9%8A%D8%B9%D9%8A</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/ليبيا</t>
+          <t>https://ar.wikipedia.org/wiki/العراق</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%88%D8%B4%D9%85_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B1%D8%AC%D8%B9_%D8%A7%D9%84%D8%A8%D8%B9%D9%8A%D8%AF_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D8%B1%D8%AD%D9%85%D9%86_%D9%85%D8%AC%D9%8A%D8%AF_%D8%A7%D9%84%D8%B1%D8%A8%D9%8A%D8%B9%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%81%D8%A4%D8%A7%D8%AF_%D8%A7%D9%84%D8%AA%D9%83%D8%B1%D9%84%D9%8A</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -697,116 +693,116 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B1%D8%AC%D8%B9_%D8%A7%D9%84%D8%A8%D8%B9%D9%8A%D8%AF_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B4%D8%B1%D8%A7%D8%B9_%D9%88%D8%A7%D9%84%D8%B9%D8%A7%D8%B5%D9%81%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%81%D8%A4%D8%A7%D8%AF_%D8%A7%D9%84%D8%AA%D9%83%D8%B1%D9%84%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AD%D9%86%D8%A7_%D9%85%D9%8A%D9%86%D9%87</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/العراق</t>
+          <t>https://ar.wikipedia.org/wiki/سوريا</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B4%D8%B1%D8%A7%D8%B9_%D9%88%D8%A7%D9%84%D8%B9%D8%A7%D8%B5%D9%81%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B2%D9%8A%D9%86%D9%8A_%D8%A8%D8%B1%D9%83%D8%A7%D8%AA_(%D8%AA%D9%88%D8%B6%D9%8A%D8%AD)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AD%D9%86%D8%A7_%D9%85%D9%8A%D9%86%D9%87</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AC%D9%85%D8%A7%D9%84_%D8%A7%D9%84%D8%BA%D9%8A%D8%B7%D8%A7%D9%86%D9%8A</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/سوريا</t>
+          <t>https://ar.wikipedia.org/wiki/مصر</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B2%D9%8A%D9%86%D9%8A_%D8%A8%D8%B1%D9%83%D8%A7%D8%AA_(%D8%AA%D9%88%D8%B6%D9%8A%D8%AD)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B3%D8%A3%D9%87%D8%A8%D9%83_%D9%85%D8%AF%D9%8A%D9%86%D8%A9_%D8%A3%D8%AE%D8%B1%D9%89_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9_%D8%AB%D9%84%D8%A7%D8%AB%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AC%D9%85%D8%A7%D9%84_%D8%A7%D9%84%D8%BA%D9%8A%D8%B7%D8%A7%D9%86%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A3%D8%AD%D9%85%D8%AF_%D8%A5%D8%A8%D8%B1%D8%A7%D9%87%D9%8A%D9%85_%D8%A7%D9%84%D9%81%D9%82%D9%8A%D9%87</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/مصر</t>
+          <t>https://ar.wikipedia.org/wiki/ليبيا</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B3%D8%A3%D9%87%D8%A8%D9%83_%D9%85%D8%AF%D9%8A%D9%86%D8%A9_%D8%A3%D8%AE%D8%B1%D9%89_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9_%D8%AB%D9%84%D8%A7%D8%AB%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A3%D9%86%D8%A7_%D8%A3%D8%AD%D9%8A%D8%A7</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A3%D8%AD%D9%85%D8%AF_%D8%A5%D8%A8%D8%B1%D8%A7%D9%87%D9%8A%D9%85_%D8%A7%D9%84%D9%81%D9%82%D9%8A%D9%87</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%84%D9%8A%D9%84%D9%89_%D8%A8%D8%B9%D9%84%D8%A8%D9%83%D9%8A</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/ليبيا</t>
+          <t>https://ar.wikipedia.org/wiki/لبنان</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A3%D9%86%D8%A7_%D8%A3%D8%AD%D9%8A%D8%A7</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%84%D8%A7_%D8%A3%D8%AD%D8%AF_%D9%8A%D9%86%D8%A7%D9%85_%D9%81%D9%8A_%D8%A7%D9%84%D8%A5%D8%B3%D9%83%D9%86%D8%AF%D8%B1%D9%8A%D8%A9</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%84%D9%8A%D9%84%D9%89_%D8%A8%D8%B9%D9%84%D8%A8%D9%83%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A5%D8%A8%D8%B1%D8%A7%D9%87%D9%8A%D9%85_%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D9%85%D8%AC%D9%8A%D8%AF</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/لبنان</t>
+          <t>https://ar.wikipedia.org/wiki/مصر</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%84%D8%A7_%D8%A3%D8%AD%D8%AF_%D9%8A%D9%86%D8%A7%D9%85_%D9%81%D9%8A_%D8%A7%D9%84%D8%A5%D8%B3%D9%83%D9%86%D8%AF%D8%B1%D9%8A%D8%A9</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%AD%D8%A8_%D9%81%D9%8A_%D8%A7%D9%84%D9%85%D9%86%D9%81%D9%89</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A5%D8%A8%D8%B1%D8%A7%D9%87%D9%8A%D9%85_%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D9%85%D8%AC%D9%8A%D8%AF</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A8%D9%87%D8%A7%D8%A1_%D8%B7%D8%A7%D9%87%D8%B1</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -817,36 +813,36 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%AD%D8%A8_%D9%81%D9%8A_%D8%A7%D9%84%D9%85%D9%86%D9%81%D9%89</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AF%D8%A7%D8%B1%D8%A7%D8%AA_%D8%A7%D9%84%D8%B4%D8%B1%D9%82</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A8%D9%87%D8%A7%D8%A1_%D8%B7%D8%A7%D9%87%D8%B1</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%86%D8%A8%D9%8A%D9%84_%D8%B3%D9%84%D9%8A%D9%85%D8%A7%D9%86</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/مصر</t>
+          <t>https://ar.wikipedia.org/wiki/سوريا</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AF%D8%A7%D8%B1%D8%A7%D8%AA_%D8%A7%D9%84%D8%B4%D8%B1%D9%82</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%88%D8%A8%D8%A7%D8%A1_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%86%D8%A8%D9%8A%D9%84_%D8%B3%D9%84%D9%8A%D9%85%D8%A7%D9%86</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%87%D8%A7%D9%86%D9%8A_%D8%A7%D9%84%D8%B1%D8%A7%D9%87%D8%A8</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -857,136 +853,136 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%88%D8%A8%D8%A7%D8%A1_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%AD%D8%B1%D8%A7%D9%85_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%87%D8%A7%D9%86%D9%8A_%D8%A7%D9%84%D8%B1%D8%A7%D9%87%D8%A8</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%8A%D9%88%D8%B3%D9%81_%D8%A5%D8%AF%D8%B1%D9%8A%D8%B3</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/سوريا</t>
+          <t>https://ar.wikipedia.org/wiki/مصر</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%AD%D8%B1%D8%A7%D9%85_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%84%D9%8A%D9%84%D8%A9_%D8%A7%D9%84%D8%B3%D9%86%D9%88%D8%A7%D8%AA_%D8%A7%D9%84%D8%B9%D8%B4%D8%B1</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%8A%D9%88%D8%B3%D9%81_%D8%A5%D8%AF%D8%B1%D9%8A%D8%B3</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%A7%D9%84%D8%B5%D8%A7%D9%84%D8%AD_%D8%A7%D9%84%D8%AC%D8%A7%D8%A8%D8%B1%D9%8A</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/مصر</t>
+          <t>https://ar.wikipedia.org/wiki/تونس</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%84%D9%8A%D9%84%D8%A9_%D8%A7%D9%84%D8%B3%D9%86%D9%88%D8%A7%D8%AA_%D8%A7%D9%84%D8%B9%D8%B4%D8%B1</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D9%88%D8%B3%D9%85_%D8%A7%D9%84%D9%87%D8%AC%D8%B1%D8%A9_%D8%A5%D9%84%D9%89_%D8%A7%D9%84%D8%B4%D9%85%D8%A7%D9%84</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%A7%D9%84%D8%B5%D8%A7%D9%84%D8%AD_%D8%A7%D9%84%D8%AC%D8%A7%D8%A8%D8%B1%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B7%D9%8A%D8%A8_%D8%B5%D8%A7%D9%84%D8%AD</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/تونس</t>
+          <t>https://ar.wikipedia.org/wiki/السودان</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D9%88%D8%B3%D9%85_%D8%A7%D9%84%D9%87%D8%AC%D8%B1%D8%A9_%D8%A5%D9%84%D9%89_%D8%A7%D9%84%D8%B4%D9%85%D8%A7%D9%84</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B0%D8%A7%D9%83%D8%B1%D8%A9_%D8%A7%D9%84%D8%AC%D8%B3%D8%AF_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B7%D9%8A%D8%A8_%D8%B5%D8%A7%D9%84%D8%AD</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A3%D8%AD%D9%84%D8%A7%D9%85_%D9%85%D8%B3%D8%AA%D8%BA%D8%A7%D9%86%D9%85%D9%8A</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/السودان</t>
+          <t>https://ar.wikipedia.org/wiki/الجزائر</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B0%D8%A7%D9%83%D8%B1%D8%A9_%D8%A7%D9%84%D8%AC%D8%B3%D8%AF_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%AE%D8%A8%D8%B2_%D8%A7%D9%84%D8%AD%D8%A7%D9%81%D9%8A</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A3%D8%AD%D9%84%D8%A7%D9%85_%D9%85%D8%B3%D8%AA%D8%BA%D8%A7%D9%86%D9%85%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%B4%D9%83%D8%B1%D9%8A</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/الجزائر</t>
+          <t>https://ar.wikipedia.org/wiki/المغرب</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%AE%D8%A8%D8%B2_%D8%A7%D9%84%D8%AD%D8%A7%D9%81%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AA%D8%B4%D8%B1%D9%8A%D9%81%D8%A9_%D8%A2%D9%84_%D8%A7%D9%84%D9%85%D8%B1</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%B4%D9%83%D8%B1%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D9%83%D8%B1%D9%8A%D9%85_%D9%86%D8%A7%D8%B5%D9%8A%D9%81</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/المغرب</t>
+          <t>https://ar.wikipedia.org/wiki/سوريا</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AA%D8%B4%D8%B1%D9%8A%D9%81%D8%A9_%D8%A2%D9%84_%D8%A7%D9%84%D9%85%D8%B1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AF%D8%A7%D8%B1_%D8%A7%D9%84%D9%85%D8%AA%D8%B9%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D9%83%D8%B1%D9%8A%D9%85_%D9%86%D8%A7%D8%B5%D9%8A%D9%81</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%88%D9%84%D9%8A%D8%AF_%D8%A5%D8%AE%D9%84%D8%A7%D8%B5%D9%8A</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -997,76 +993,76 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AF%D8%A7%D8%B1_%D8%A7%D9%84%D9%85%D8%AA%D8%B9%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B7%D9%88%D8%A7%D8%AD%D9%8A%D9%86_%D8%A8%D9%8A%D8%B1%D9%88%D8%AA</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%88%D9%84%D9%8A%D8%AF_%D8%A5%D8%AE%D9%84%D8%A7%D8%B5%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AA%D9%88%D9%81%D9%8A%D9%82_%D9%8A%D9%88%D8%B3%D9%81_%D8%B9%D9%88%D8%A7%D8%AF</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/سوريا</t>
+          <t>https://ar.wikipedia.org/wiki/لبنان</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B7%D9%88%D8%A7%D8%AD%D9%8A%D9%86_%D8%A8%D9%8A%D8%B1%D9%88%D8%AA</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%A3%D9%81%D9%8A%D8%A7%D9%84_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AA%D9%88%D9%81%D9%8A%D9%82_%D9%8A%D9%88%D8%B3%D9%81_%D8%B9%D9%88%D8%A7%D8%AF</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%81%D8%AA%D8%AD%D9%8A_%D8%BA%D8%A7%D9%86%D9%85</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/لبنان</t>
+          <t>https://ar.wikipedia.org/wiki/مصر</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%A3%D9%81%D9%8A%D8%A7%D9%84_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%86%D8%AC%D8%B1%D8%A7%D9%86_%D8%AA%D8%AD%D8%AA_%D8%A7%D9%84%D8%B5%D9%81%D8%B1</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%81%D8%AA%D8%AD%D9%8A_%D8%BA%D8%A7%D9%86%D9%85</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%8A%D8%AD%D9%8A%D9%89_%D9%8A%D8%AE%D9%84%D9%81</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/مصر</t>
+          <t>https://ar.wikipedia.org/wiki/فلسطين</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%86%D8%AC%D8%B1%D8%A7%D9%86_%D8%AA%D8%AD%D8%AA_%D8%A7%D9%84%D8%B5%D9%81%D8%B1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B9%D8%B4%D8%A7%D9%82_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%8A%D8%AD%D9%8A%D9%89_%D9%8A%D8%AE%D9%84%D9%81</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B1%D8%B4%D8%A7%D8%AF_%D8%A3%D8%A8%D9%88_%D8%B4%D8%A7%D9%88%D8%B1</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1077,96 +1073,96 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B9%D8%B4%D8%A7%D9%82_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%A7%D8%B9%D8%AA%D8%B1%D8%A7%D9%81_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B1%D8%B4%D8%A7%D8%AF_%D8%A3%D8%A8%D9%88_%D8%B4%D8%A7%D9%88%D8%B1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B9%D9%84%D9%8A_%D8%A3%D8%A8%D9%88_%D8%A7%D9%84%D8%B1%D9%8A%D8%B4</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/فلسطين</t>
+          <t>https://ar.wikipedia.org/wiki/الإمارات العربية المتحدة</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%A7%D8%B9%D8%AA%D8%B1%D8%A7%D9%81_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%86%D8%AE%D9%84%D8%A9_%D9%88%D8%A7%D9%84%D8%AC%D9%8A%D8%B1%D8%A7%D9%86_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B9%D9%84%D9%8A_%D8%A3%D8%A8%D9%88_%D8%A7%D9%84%D8%B1%D9%8A%D8%B4</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%BA%D8%A7%D8%A6%D8%A8_%D8%B7%D8%B9%D9%85%D8%A9_%D9%81%D8%B1%D9%85%D8%A7%D9%86</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/الإمارات العربية المتحدة</t>
+          <t>https://ar.wikipedia.org/wiki/العراق</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%86%D8%AE%D9%84%D8%A9_%D9%88%D8%A7%D9%84%D8%AC%D9%8A%D8%B1%D8%A7%D9%86_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B9%D8%B5%D9%81%D9%88%D8%B1%D9%8A%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%BA%D8%A7%D8%A6%D8%A8_%D8%B7%D8%B9%D9%85%D8%A9_%D9%81%D8%B1%D9%85%D8%A7%D9%86</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%BA%D8%A7%D8%B2%D9%8A_%D8%A7%D9%84%D9%82%D8%B5%D9%8A%D8%A8%D9%8A</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/العراق</t>
+          <t>https://ar.wikipedia.org/wiki/السعودية</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B9%D8%B5%D9%81%D9%88%D8%B1%D9%8A%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%82%D9%86%D8%AF%D9%8A%D9%84_%D8%A3%D9%85_%D9%87%D8%A7%D8%B4%D9%85_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%BA%D8%A7%D8%B2%D9%8A_%D8%A7%D9%84%D9%82%D8%B5%D9%8A%D8%A8%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%8A%D8%AD%D9%8A%D9%89_%D8%AD%D9%82%D9%8A</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/السعودية</t>
+          <t>https://ar.wikipedia.org/wiki/مصر</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%82%D9%86%D8%AF%D9%8A%D9%84_%D8%A3%D9%85_%D9%87%D8%A7%D8%B4%D9%85_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B9%D9%88%D8%AF%D8%A9_%D8%A5%D9%84%D9%89_%D8%A7%D9%84%D9%85%D9%86%D9%81%D9%89</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%8A%D8%AD%D9%8A%D9%89_%D8%AD%D9%82%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A3%D8%A8%D9%88_%D8%A7%D9%84%D9%85%D8%B9%D8%A7%D8%B7%D9%8A_%D8%A3%D8%A8%D9%88_%D8%A7%D9%84%D9%86%D8%AC%D8%A7</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1177,16 +1173,16 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B9%D9%88%D8%AF%D8%A9_%D8%A5%D9%84%D9%89_%D8%A7%D9%84%D9%85%D9%86%D9%81%D9%89</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%88%D9%83%D8%A7%D9%84%D8%A9_%D8%B9%D8%B7%D9%8A%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A3%D8%A8%D9%88_%D8%A7%D9%84%D9%85%D8%B9%D8%A7%D8%B7%D9%8A_%D8%A3%D8%A8%D9%88_%D8%A7%D9%84%D9%86%D8%AC%D8%A7</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AE%D9%8A%D8%B1%D9%8A_%D8%B4%D9%84%D8%A8%D9%8A</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1197,96 +1193,96 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%88%D9%83%D8%A7%D9%84%D8%A9_%D8%B9%D8%B7%D9%8A%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AA%D9%85%D8%A7%D8%B3_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AE%D9%8A%D8%B1%D9%8A_%D8%B4%D9%84%D8%A8%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%B1%D9%88%D8%B3%D9%8A%D8%A9_%D8%A7%D9%84%D9%86%D8%A7%D9%84%D9%88%D8%AA%D9%8A</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/مصر</t>
+          <t>https://ar.wikipedia.org/wiki/تونس</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AA%D9%85%D8%A7%D8%B3_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B3%D9%84%D8%B7%D8%A7%D9%86%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%B1%D9%88%D8%B3%D9%8A%D8%A9_%D8%A7%D9%84%D9%86%D8%A7%D9%84%D9%88%D8%AA%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%BA%D8%A7%D9%84%D8%A8_%D9%87%D9%84%D8%B3%D8%A7</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/تونس</t>
+          <t>https://ar.wikipedia.org/wiki/الأردن</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B3%D9%84%D8%B7%D8%A7%D9%86%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%A7%D9%84%D9%83_%D8%A7%D9%84%D8%AD%D8%B2%D9%8A%D9%86_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%BA%D8%A7%D9%84%D8%A8_%D9%87%D9%84%D8%B3%D8%A7</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A5%D8%A8%D8%B1%D8%A7%D9%87%D9%8A%D9%85_%D8%A3%D8%B5%D9%84%D8%A7%D9%86</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/الأردن</t>
+          <t>https://ar.wikipedia.org/wiki/مصر</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%A7%D9%84%D9%83_%D8%A7%D9%84%D8%AD%D8%B2%D9%8A%D9%86_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A8%D8%A7%D8%A8_%D8%A7%D9%84%D8%B4%D9%85%D8%B3_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A5%D8%A8%D8%B1%D8%A7%D9%87%D9%8A%D9%85_%D8%A3%D8%B5%D9%84%D8%A7%D9%86</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A5%D9%84%D9%8A%D8%A7%D8%B3_%D8%AE%D9%88%D8%B1%D9%8A</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/مصر</t>
+          <t>https://ar.wikipedia.org/wiki/لبنان</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A8%D8%A7%D8%A8_%D8%A7%D9%84%D8%B4%D9%85%D8%B3_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%AD%D9%8A_%D8%A7%D9%84%D9%84%D8%A7%D8%AA%D9%8A%D9%86%D9%8A_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A5%D9%84%D9%8A%D8%A7%D8%B3_%D8%AE%D9%88%D8%B1%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B3%D9%87%D9%8A%D9%84_%D8%A5%D8%AF%D8%B1%D9%8A%D8%B3</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1297,76 +1293,76 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%AD%D9%8A_%D8%A7%D9%84%D9%84%D8%A7%D8%AA%D9%8A%D9%86%D9%8A_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B9%D9%88%D8%AF%D8%A9_%D8%A7%D9%84%D8%B1%D9%88%D8%AD_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B3%D9%87%D9%8A%D9%84_%D8%A5%D8%AF%D8%B1%D9%8A%D8%B3</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AA%D9%88%D9%81%D9%8A%D9%82_%D8%A7%D9%84%D8%AD%D9%83%D9%8A%D9%85</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/لبنان</t>
+          <t>https://ar.wikipedia.org/wiki/مصر</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B9%D9%88%D8%AF%D8%A9_%D8%A7%D9%84%D8%B1%D9%88%D8%AD_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B1%D9%87%D9%8A%D9%86%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AA%D9%88%D9%81%D9%8A%D9%82_%D8%A7%D9%84%D8%AD%D9%83%D9%8A%D9%85</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B2%D9%8A%D8%AF_%D9%85%D8%B7%D9%8A%D8%B9_%D8%AF%D9%85%D8%A7%D8%AC</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/مصر</t>
+          <t>https://ar.wikipedia.org/wiki/اليمن</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B1%D9%87%D9%8A%D9%86%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%84%D8%B9%D8%A8%D8%A9_%D8%A7%D9%84%D9%86%D8%B3%D9%8A%D8%A7%D9%86</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B2%D9%8A%D8%AF_%D9%85%D8%B7%D9%8A%D8%B9_%D8%AF%D9%85%D8%A7%D8%AC</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%A8%D8%B1%D8%A7%D8%AF%D8%A9</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/اليمن</t>
+          <t>https://ar.wikipedia.org/wiki/المغرب</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%84%D8%B9%D8%A8%D8%A9_%D8%A7%D9%84%D9%86%D8%B3%D9%8A%D8%A7%D9%86</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B1%D9%8A%D8%AD_%D8%A7%D9%84%D8%B4%D8%AA%D9%88%D9%8A%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%A8%D8%B1%D8%A7%D8%AF%D8%A9</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%A8%D8%A7%D8%B1%D9%83_%D8%B1%D8%A8%D9%8A%D8%B9</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1377,276 +1373,276 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B1%D9%8A%D8%AD_%D8%A7%D9%84%D8%B4%D8%AA%D9%88%D9%8A%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%AF%D8%A7%D8%B1_%D8%A7%D9%84%D8%A8%D8%A7%D8%B4%D8%A7_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%A8%D8%A7%D8%B1%D9%83_%D8%B1%D8%A8%D9%8A%D8%B9</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AD%D8%B3%D9%86_%D9%86%D8%B5%D8%B1</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/المغرب</t>
+          <t>https://ar.wikipedia.org/wiki/تونس</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%AF%D8%A7%D8%B1_%D8%A7%D9%84%D8%A8%D8%A7%D8%B4%D8%A7_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D9%85%D8%AF%D9%8A%D9%86%D8%A9_%D8%A7%D9%84%D8%B1%D9%8A%D8%A7%D8%AD_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AD%D8%B3%D9%86_%D9%86%D8%B5%D8%B1</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D9%88%D8%B3%D9%89_%D9%88%D9%84%D8%AF_%D8%A7%D8%A8%D9%86%D9%88</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/تونس</t>
+          <t>https://ar.wikipedia.org/wiki/موريتانيا</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D9%85%D8%AF%D9%8A%D9%86%D8%A9_%D8%A7%D9%84%D8%B1%D9%8A%D8%A7%D8%AD_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A3%D8%A8%D9%88%D8%A7%D8%A8_%D8%A7%D9%84%D8%B1%D9%88%D8%AD_%D8%A7%D9%84%D8%B3%D8%A8%D8%B9%D8%A9&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D9%88%D8%B3%D9%89_%D9%88%D9%84%D8%AF_%D8%A7%D8%A8%D9%86%D9%88</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A3%D9%8A%D9%88%D8%A8_%D8%A7%D9%84%D8%AD%D8%AC%D9%84%D9%8A</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/موريتانيا</t>
+          <t>https://ar.wikipedia.org/wiki/سوريا</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A3%D8%A8%D9%88%D8%A7%D8%A8_%D8%A7%D9%84%D8%B1%D9%88%D8%AD_%D8%A7%D9%84%D8%B3%D8%A8%D8%B9%D8%A9&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A3%D9%8A%D8%A7%D9%85_%D8%A7%D9%84%D8%A5%D9%86%D8%B3%D8%A7%D9%86_%D8%A7%D9%84%D8%B3%D8%A8%D8%B9%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A3%D9%8A%D9%88%D8%A8_%D8%A7%D9%84%D8%AD%D8%AC%D9%84%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D8%AD%D9%83%D9%8A%D9%85_%D9%82%D8%A7%D8%B3%D9%85</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/سوريا</t>
+          <t>https://ar.wikipedia.org/wiki/مصر</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A3%D9%8A%D8%A7%D9%85_%D8%A7%D9%84%D8%A5%D9%86%D8%B3%D8%A7%D9%86_%D8%A7%D9%84%D8%B3%D8%A8%D8%B9%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%B7%D8%A7%D8%A6%D8%B1_%D8%A7%D9%84%D8%AD%D9%88%D9%85_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D8%AD%D9%83%D9%8A%D9%85_%D9%82%D8%A7%D8%B3%D9%85</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AD%D9%84%D9%8A%D9%85_%D8%A8%D8%B1%D9%83%D8%A7%D8%AA</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/مصر</t>
+          <t>https://ar.wikipedia.org/wiki/سوريا</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%B7%D8%A7%D8%A6%D8%B1_%D8%A7%D9%84%D8%AD%D9%88%D9%85_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AD%D9%83%D8%A7%D9%8A%D8%A9_%D8%B2%D9%87%D8%B1%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AD%D9%84%D9%8A%D9%85_%D8%A8%D8%B1%D9%83%D8%A7%D8%AA</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AD%D9%86%D8%A7%D9%86_%D8%A7%D9%84%D8%B4%D9%8A%D8%AE</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/سوريا</t>
+          <t>https://ar.wikipedia.org/wiki/لبنان</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AD%D9%83%D8%A7%D9%8A%D8%A9_%D8%B2%D9%87%D8%B1%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B1%D9%8A%D8%AD_%D8%A7%D9%84%D8%AC%D9%86%D9%88%D8%A8_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AD%D9%86%D8%A7%D9%86_%D8%A7%D9%84%D8%B4%D9%8A%D8%AE</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D8%AD%D9%85%D9%8A%D8%AF_%D8%A8%D9%86_%D9%87%D8%AF%D9%88%D9%82%D8%A9</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/لبنان</t>
+          <t>https://ar.wikipedia.org/wiki/الجزائر</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B1%D9%8A%D8%AD_%D8%A7%D9%84%D8%AC%D9%86%D9%88%D8%A8_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%81%D8%B1%D8%AF%D9%88%D8%B3_%D8%A7%D9%84%D8%AC%D9%86%D9%88%D9%86_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D8%AD%D9%85%D9%8A%D8%AF_%D8%A8%D9%86_%D9%87%D8%AF%D9%88%D9%82%D8%A9</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A3%D8%AD%D9%85%D8%AF_%D9%8A%D9%88%D8%B3%D9%81_%D8%AF%D8%A7%D9%88%D9%88%D8%AF</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/الجزائر</t>
+          <t>https://ar.wikipedia.org/wiki/سوريا</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%81%D8%B1%D8%AF%D9%88%D8%B3_%D8%A7%D9%84%D8%AC%D9%86%D9%88%D9%86_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D9%88%D8%B3%D9%85%D9%8A%D8%A9_%D8%AA%D8%AE%D8%B1%D8%AC_%D9%85%D9%86_%D8%A7%D9%84%D8%A8%D8%AD%D8%B1_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A3%D8%AD%D9%85%D8%AF_%D9%8A%D9%88%D8%B3%D9%81_%D8%AF%D8%A7%D9%88%D9%88%D8%AF</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%84%D9%8A%D9%84%D9%89_%D8%A7%D9%84%D8%B9%D8%AB%D9%85%D8%A7%D9%86</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/سوريا</t>
+          <t>https://ar.wikipedia.org/wiki/الكويت</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D9%88%D8%B3%D9%85%D9%8A%D8%A9_%D8%AA%D8%AE%D8%B1%D8%AC_%D9%85%D9%86_%D8%A7%D9%84%D8%A8%D8%AD%D8%B1_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D8%B9%D8%AA%D8%B1%D8%A7%D9%81%D8%A7%D8%AA_%D9%83%D8%A7%D8%AA%D9%85_%D8%B5%D9%88%D8%AA_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%84%D9%8A%D9%84%D9%89_%D8%A7%D9%84%D8%B9%D8%AB%D9%85%D8%A7%D9%86</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%A4%D9%86%D8%B3_%D8%A7%D9%84%D8%B1%D8%B2%D8%A7%D8%B2</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/الكويت</t>
+          <t>https://ar.wikipedia.org/wiki/الأردن</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D8%B9%D8%AA%D8%B1%D8%A7%D9%81%D8%A7%D8%AA_%D9%83%D8%A7%D8%AA%D9%85_%D8%B5%D9%88%D8%AA_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%B1%D8%A8%D8%A7%D8%B9%D9%8A%D8%A9_%D8%A8%D8%AD%D8%B1%D9%8A_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%A4%D9%86%D8%B3_%D8%A7%D9%84%D8%B1%D8%B2%D8%A7%D8%B2</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%AC%D8%A8%D8%B1%D9%8A%D9%84_(%D8%AA%D9%88%D8%B6%D9%8A%D8%AD)</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/الأردن</t>
+          <t>https://ar.wikipedia.org/wiki/مصر</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%B1%D8%A8%D8%A7%D8%B9%D9%8A%D8%A9_%D8%A8%D8%AD%D8%B1%D9%8A_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%B5%D9%86%D8%B9%D8%A7%D8%A1_%D9%85%D8%AF%D9%8A%D9%86%D8%A9_%D9%85%D9%81%D8%AA%D9%88%D8%AD%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%AC%D8%A8%D8%B1%D9%8A%D9%84_(%D8%AA%D9%88%D8%B6%D9%8A%D8%AD)</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D9%88%D9%84%D9%8A</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/مصر</t>
+          <t>https://ar.wikipedia.org/wiki/اليمن</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%B5%D9%86%D8%B9%D8%A7%D8%A1_%D9%85%D8%AF%D9%8A%D9%86%D8%A9_%D9%85%D9%81%D8%AA%D9%88%D8%AD%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AB%D9%84%D8%A7%D8%AB%D9%8A%D8%A9_%D8%BA%D8%B1%D9%86%D8%A7%D8%B7%D8%A9</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D9%88%D9%84%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B1%D8%B6%D9%88%D9%89_%D8%B9%D8%A7%D8%B4%D9%88%D8%B1</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/اليمن</t>
+          <t>https://ar.wikipedia.org/wiki/مصر</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AB%D9%84%D8%A7%D8%AB%D9%8A%D8%A9_%D8%BA%D8%B1%D9%86%D8%A7%D8%B7%D8%A9</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AF%D8%B9%D8%A7%D8%A1_%D8%A7%D9%84%D9%83%D8%B1%D9%88%D8%A7%D9%86_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B1%D8%B6%D9%88%D9%89_%D8%B9%D8%A7%D8%B4%D9%88%D8%B1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B7%D9%87_%D8%AD%D8%B3%D9%8A%D9%86</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1657,16 +1653,16 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AF%D8%B9%D8%A7%D8%A1_%D8%A7%D9%84%D9%83%D8%B1%D9%88%D8%A7%D9%86_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D9%81%D8%B3%D8%A7%D8%AF_%D8%A7%D9%84%D8%A7%D9%85%D9%83%D9%86%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B7%D9%87_%D8%AD%D8%B3%D9%8A%D9%86</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B5%D8%A8%D8%B1%D9%8A_%D9%85%D9%88%D8%B3%D9%89</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1677,16 +1673,16 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D9%81%D8%B3%D8%A7%D8%AF_%D8%A7%D9%84%D8%A7%D9%85%D9%83%D9%86%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B3%D9%82%D8%A7_%D9%85%D8%A7%D8%AA_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B5%D8%A8%D8%B1%D9%8A_%D9%85%D9%88%D8%B3%D9%89</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%8A%D9%88%D8%B3%D9%81_%D8%A7%D9%84%D8%B3%D8%A8%D8%A7%D8%B9%D9%8A</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -1697,16 +1693,16 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B3%D9%82%D8%A7_%D9%85%D8%A7%D8%AA_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%AA%D8%BA%D8%B1%D9%8A%D8%A8%D9%87_%D8%A8%D9%86%D9%8A_%D8%AD%D8%AA%D8%AD%D9%88%D8%AA_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%8A%D9%88%D8%B3%D9%81_%D8%A7%D9%84%D8%B3%D8%A8%D8%A7%D8%B9%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AC%D9%8A%D8%AF_%D8%B7%D9%88%D8%A8%D9%8A%D8%A7</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -1717,16 +1713,16 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%AA%D8%BA%D8%B1%D9%8A%D8%A8%D9%87_%D8%A8%D9%86%D9%8A_%D8%AD%D8%AA%D8%AD%D9%88%D8%AA_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A8%D8%B9%D8%AF_%D8%A7%D9%84%D8%BA%D8%B1%D9%88%D8%A8_(%D9%83%D8%AA%D8%A7%D8%A8)</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AC%D9%8A%D8%AF_%D8%B7%D9%88%D8%A8%D9%8A%D8%A7</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D8%AD%D9%84%D9%8A%D9%85_%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D9%84%D9%87</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -1737,96 +1733,96 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A8%D8%B9%D8%AF_%D8%A7%D9%84%D8%BA%D8%B1%D9%88%D8%A8_(%D9%83%D8%AA%D8%A7%D8%A8)</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%82%D9%84%D9%88%D8%A8_%D8%B9%D9%84%D9%89_%D8%A7%D9%84%D8%A3%D8%B3%D9%84%D8%A7%D9%83</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D8%AD%D9%84%D9%8A%D9%85_%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D9%84%D9%87</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D8%B3%D9%84%D8%A7%D9%85_%D8%A7%D9%84%D8%B9%D8%AC%D9%8A%D9%84%D9%8A</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/مصر</t>
+          <t>https://ar.wikipedia.org/wiki/سوريا</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%82%D9%84%D9%88%D8%A8_%D8%B9%D9%84%D9%89_%D8%A7%D9%84%D8%A3%D8%B3%D9%84%D8%A7%D9%83</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A7%D8%A6%D8%B4%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D8%B3%D9%84%D8%A7%D9%85_%D8%A7%D9%84%D8%B9%D8%AC%D9%8A%D9%84%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%A8%D8%B4%D9%8A%D8%B1_%D8%A8%D9%86_%D8%B3%D9%84%D8%A7%D9%85%D8%A9</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/سوريا</t>
+          <t>https://ar.wikipedia.org/wiki/تونس</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A7%D8%A6%D8%B4%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B8%D9%84_%D9%88%D8%A7%D9%84%D8%B5%D8%AF%D9%89_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%A8%D8%B4%D9%8A%D8%B1_%D8%A8%D9%86_%D8%B3%D9%84%D8%A7%D9%85%D8%A9</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%8A%D9%88%D8%B3%D9%81_%D8%AD%D8%A8%D8%B4%D9%8A_%D8%A7%D9%84%D8%A3%D8%B4%D9%82%D8%B1</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/تونس</t>
+          <t>https://ar.wikipedia.org/wiki/لبنان</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B8%D9%84_%D9%88%D8%A7%D9%84%D8%B5%D8%AF%D9%89_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%AF%D9%82%D9%84%D8%A9_%D9%81%D9%8A_%D8%B9%D8%B1%D8%A7%D8%AC%D9%8A%D9%86%D9%87%D8%A7_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%8A%D9%88%D8%B3%D9%81_%D8%AD%D8%A8%D8%B4%D9%8A_%D8%A7%D9%84%D8%A3%D8%B4%D9%82%D8%B1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A8%D8%B4%D9%8A%D8%B1_%D8%AE%D8%B1%D9%8A%D9%81</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/لبنان</t>
+          <t>https://ar.wikipedia.org/wiki/تونس</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%AF%D9%82%D9%84%D8%A9_%D9%81%D9%8A_%D8%B9%D8%B1%D8%A7%D8%AC%D9%8A%D9%86%D9%87%D8%A7_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%86%D8%AE%D8%A7%D8%B3_(%D9%83%D8%AA%D8%A7%D8%A8)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A8%D8%B4%D9%8A%D8%B1_%D8%AE%D8%B1%D9%8A%D9%81</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B5%D9%84%D8%A7%D8%AD_%D8%A7%D9%84%D8%AF%D9%8A%D9%86_%D8%A8%D9%88%D8%AC%D8%A7%D9%87</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -1837,436 +1833,436 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%86%D8%AE%D8%A7%D8%B3_(%D9%83%D8%AA%D8%A7%D8%A8)</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A8%D8%A7%D8%A8_%D8%A7%D9%84%D8%B3%D8%A7%D8%AD%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B5%D9%84%D8%A7%D8%AD_%D8%A7%D9%84%D8%AF%D9%8A%D9%86_%D8%A8%D9%88%D8%AC%D8%A7%D9%87</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B3%D8%AD%D8%B1_%D8%AE%D9%84%D9%8A%D9%81%D8%A9</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/تونس</t>
+          <t>https://ar.wikipedia.org/wiki/فلسطين</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A8%D8%A7%D8%A8_%D8%A7%D9%84%D8%B3%D8%A7%D8%AD%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%B3%D8%A7%D8%A8%D8%B9_%D8%A7%D9%8A%D8%A7%D9%85_%D8%A7%D9%84%D8%AE%D9%84%D9%82_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B3%D8%AD%D8%B1_%D8%AE%D9%84%D9%8A%D9%81%D8%A9</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D8%AE%D8%A7%D9%84%D9%82_%D8%A7%D9%84%D8%B1%D9%83%D8%A7%D8%A8%D9%8A</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/فلسطين</t>
+          <t>https://ar.wikipedia.org/wiki/العراق</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%B3%D8%A7%D8%A8%D8%B9_%D8%A7%D9%8A%D8%A7%D9%85_%D8%A7%D9%84%D8%AE%D9%84%D9%82_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%B4%D9%8A%D8%A1_%D9%85%D9%86_%D8%A7%D9%84%D8%AE%D9%88%D9%81_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D8%AE%D8%A7%D9%84%D9%82_%D8%A7%D9%84%D8%B1%D9%83%D8%A7%D8%A8%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AB%D8%B1%D9%88%D8%AA_%D8%A3%D8%A8%D8%A7%D8%B8%D8%A9</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/العراق</t>
+          <t>https://ar.wikipedia.org/wiki/مصر</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%B4%D9%8A%D8%A1_%D9%85%D9%86_%D8%A7%D9%84%D8%AE%D9%88%D9%81_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%84%D8%A7%D8%B2_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AB%D8%B1%D9%88%D8%AA_%D8%A3%D8%A8%D8%A7%D8%B8%D8%A9</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B7%D8%A7%D9%87%D8%B1_%D9%88%D8%B7%D8%A7%D8%B1</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/مصر</t>
+          <t>https://ar.wikipedia.org/wiki/الجزائر</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%84%D8%A7%D8%B2_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%85%D8%B1%D8%A3%D8%A9_%D9%88%D8%A7%D9%84%D9%88%D8%B1%D8%AF%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B7%D8%A7%D9%87%D8%B1_%D9%88%D8%B7%D8%A7%D8%B1</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%B2%D9%81%D8%B2%D8%A7%D9%81</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/الجزائر</t>
+          <t>https://ar.wikipedia.org/wiki/المغرب</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%85%D8%B1%D8%A3%D8%A9_%D9%88%D8%A7%D9%84%D9%88%D8%B1%D8%AF%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A3%D9%84%D9%81_%D8%B9%D8%A7%D9%85_%D9%88%D8%B9%D8%A7%D9%85_%D9%85%D9%86_%D8%A7%D9%84%D8%AD%D9%86%D9%8A%D9%86_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%B2%D9%81%D8%B2%D8%A7%D9%81</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B1%D8%B4%D9%8A%D8%AF_%D8%A8%D9%88%D8%AC%D8%AF%D8%B1%D8%A9</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/المغرب</t>
+          <t>https://ar.wikipedia.org/wiki/الجزائر</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A3%D9%84%D9%81_%D8%B9%D8%A7%D9%85_%D9%88%D8%B9%D8%A7%D9%85_%D9%85%D9%86_%D8%A7%D9%84%D8%AD%D9%86%D9%8A%D9%86_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%82%D8%A8%D8%B1_%D8%A7%D9%84%D9%85%D8%AC%D9%87%D9%88%D9%84_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B1%D8%B4%D9%8A%D8%AF_%D8%A8%D9%88%D8%AC%D8%AF%D8%B1%D8%A9</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A3%D8%AD%D9%85%D8%AF_%D8%A8%D9%86_%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D9%82%D8%A7%D8%AF%D8%B1</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/الجزائر</t>
+          <t>https://ar.wikipedia.org/wiki/موريتانيا</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%82%D8%A8%D8%B1_%D8%A7%D9%84%D9%85%D8%AC%D9%87%D9%88%D9%84_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%A7%D8%BA%D8%AA%D9%8A%D8%A7%D9%84_%D9%88%D8%A7%D9%84%D8%BA%D8%B6%D8%A8_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A3%D8%AD%D9%85%D8%AF_%D8%A8%D9%86_%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D9%82%D8%A7%D8%AF%D8%B1</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D9%88%D9%81%D9%82_%D8%AE%D8%B6%D8%B1</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/موريتانيا</t>
+          <t>https://ar.wikipedia.org/wiki/العراق</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%A7%D8%BA%D8%AA%D9%8A%D8%A7%D9%84_%D9%88%D8%A7%D9%84%D8%BA%D8%B6%D8%A8_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A7%D9%84%D8%AF%D9%88%D8%A7%D9%85%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D9%88%D9%81%D9%82_%D8%AE%D8%B6%D8%B1</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%82%D9%85%D8%B1_%D9%83%D9%8A%D9%84%D8%A7%D9%86%D9%8A</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/العراق</t>
+          <t>https://ar.wikipedia.org/wiki/سوريا</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A7%D9%84%D8%AF%D9%88%D8%A7%D9%85%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A7%D9%84%D8%AD%D8%B5%D8%A7%D8%B1_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%82%D9%85%D8%B1_%D9%83%D9%8A%D9%84%D8%A7%D9%86%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%81%D9%88%D8%B2%D9%8A%D8%A9_%D8%B1%D8%B4%D9%8A%D8%AF</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/سوريا</t>
+          <t>https://ar.wikipedia.org/wiki/البحرين</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A7%D9%84%D8%AD%D8%B5%D8%A7%D8%B1_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%81%D9%8A_%D8%A8%D9%8A%D8%AA%D9%86%D8%A7_%D8%B1%D8%AC%D9%84_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%81%D9%88%D8%B2%D9%8A%D8%A9_%D8%B1%D8%B4%D9%8A%D8%AF</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A5%D8%AD%D8%B3%D8%A7%D9%86_%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D9%82%D8%AF%D9%88%D8%B3</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/البحرين</t>
+          <t>https://ar.wikipedia.org/wiki/مصر</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%81%D9%8A_%D8%A8%D9%8A%D8%AA%D9%86%D8%A7_%D8%B1%D8%AC%D9%84_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%B1%D9%85%D9%88%D8%B2_%D8%B9%D8%B5%D8%B1%D9%8A%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A5%D8%AD%D8%B3%D8%A7%D9%86_%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D9%82%D8%AF%D9%88%D8%B3</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AE%D8%B6%D9%8A%D8%B1_%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D8%A3%D9%85%D9%8A%D8%B1</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/مصر</t>
+          <t>https://ar.wikipedia.org/wiki/العراق</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%B1%D9%85%D9%88%D8%B2_%D8%B9%D8%B5%D8%B1%D9%8A%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D9%88%D9%86%D8%B5%D9%8A%D8%A8%D9%8A_%D9%85%D9%86_%D8%A7%D9%84%D8%A7%D9%81%D9%82_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AE%D8%B6%D9%8A%D8%B1_%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D8%A3%D9%85%D9%8A%D8%B1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D9%82%D8%A7%D8%AF%D8%B1_%D8%A8%D9%86_%D8%A7%D9%84%D8%B4%D9%8A%D8%AE</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/العراق</t>
+          <t>https://ar.wikipedia.org/wiki/تونس</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D9%88%D9%86%D8%B5%D9%8A%D8%A8%D9%8A_%D9%85%D9%86_%D8%A7%D9%84%D8%A7%D9%81%D9%82_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AC%D9%86%D9%88%D9%86_%D8%A7%D9%84%D8%AD%D9%83%D9%85_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D9%82%D8%A7%D8%AF%D8%B1_%D8%A8%D9%86_%D8%A7%D9%84%D8%B4%D9%8A%D8%AE</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A8%D9%86%D8%B3%D8%A7%D9%84%D9%85_%D8%AD%D9%85%D9%8A%D8%B4</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/تونس</t>
+          <t>https://ar.wikipedia.org/wiki/المغرب</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AC%D9%86%D9%88%D9%86_%D8%A7%D9%84%D8%AD%D9%83%D9%85_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A7%D9%84%D8%AE%D9%85%D8%A7%D8%B3%D9%8A%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A8%D9%86%D8%B3%D8%A7%D9%84%D9%85_%D8%AD%D9%85%D9%8A%D8%B4</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A5%D8%B3%D9%85%D8%A7%D8%B9%D9%8A%D9%84_%D9%81%D9%87%D8%AF_%D8%A5%D8%B3%D9%85%D8%A7%D8%B9%D9%8A%D9%84</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/المغرب</t>
+          <t>https://ar.wikipedia.org/wiki/الكويت</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A7%D9%84%D8%AE%D9%85%D8%A7%D8%B3%D9%8A%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A3%D8%AC%D9%86%D8%AD%D8%A9_%D8%A7%D9%84%D8%AA%D9%8A%D9%87_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A5%D8%B3%D9%85%D8%A7%D8%B9%D9%8A%D9%84_%D9%81%D9%87%D8%AF_%D8%A5%D8%B3%D9%85%D8%A7%D8%B9%D9%8A%D9%84</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%AC%D9%88%D8%A7%D8%AF_%D8%A7%D9%84%D8%B5%D9%8A%D8%AF%D8%A7%D9%88%D9%8A&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/الكويت</t>
+          <t>https://ar.wikipedia.org/wiki/لبنان</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A3%D8%AC%D9%86%D8%AD%D8%A9_%D8%A7%D9%84%D8%AA%D9%8A%D9%87_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A7%D9%8A%D8%A7%D9%85_%D8%A7%D9%84%D8%B1%D9%85%D8%A7%D8%AF_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%AC%D9%88%D8%A7%D8%AF_%D8%A7%D9%84%D8%B5%D9%8A%D8%AF%D8%A7%D9%88%D9%8A&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%B9%D8%B2_%D8%A7%D9%84%D8%AF%D9%8A%D9%86_%D8%A7%D9%84%D8%AA%D8%A7%D8%B2%D9%8A</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/لبنان</t>
+          <t>https://ar.wikipedia.org/wiki/المغرب</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A7%D9%8A%D8%A7%D9%85_%D8%A7%D9%84%D8%B1%D9%85%D8%A7%D8%AF_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%B1%D8%A3%D8%B3_%D8%A8%D9%8A%D8%B1%D9%88%D8%AA_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%B9%D8%B2_%D8%A7%D9%84%D8%AF%D9%8A%D9%86_%D8%A7%D9%84%D8%AA%D8%A7%D8%B2%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%8A%D8%A7%D8%B3%D9%8A%D9%86_%D8%B1%D9%81%D8%A7%D8%B9%D9%8A%D8%A9</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/المغرب</t>
+          <t>https://ar.wikipedia.org/wiki/سوريا</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%B1%D8%A3%D8%B3_%D8%A8%D9%8A%D8%B1%D9%88%D8%AA_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B9%D9%8A%D9%86_%D8%A7%D9%84%D8%B4%D9%85%D8%B3_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%8A%D8%A7%D8%B3%D9%8A%D9%86_%D8%B1%D9%81%D8%A7%D8%B9%D9%8A%D8%A9</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%AE%D9%84%D9%8A%D9%81%D8%A9_%D8%AD%D8%B3%D9%8A%D9%86_%D9%85%D8%B5%D8%B7%D9%81%D9%8A&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/سوريا</t>
+          <t>https://ar.wikipedia.org/wiki/ليبيا</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B9%D9%8A%D9%86_%D8%A7%D9%84%D8%B4%D9%85%D8%B3_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%84%D9%88%D9%86%D8%AC%D8%A9_%D9%88%D8%A7%D9%84%D8%BA%D9%88%D9%84_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%AE%D9%84%D9%8A%D9%81%D8%A9_%D8%AD%D8%B3%D9%8A%D9%86_%D9%85%D8%B5%D8%B7%D9%81%D9%8A&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B2%D9%87%D9%88%D8%B1_%D9%88%D9%86%D9%8A%D8%B3%D9%8A</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/ليبيا</t>
+          <t>https://ar.wikipedia.org/wiki/الجزائر</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%84%D9%88%D9%86%D8%AC%D8%A9_%D9%88%D8%A7%D9%84%D8%BA%D9%88%D9%84_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B5%D8%AE%D8%A8_%D8%A7%D9%84%D8%A8%D8%AD%D9%8A%D8%B1%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B2%D9%87%D9%88%D8%B1_%D9%88%D9%86%D9%8A%D8%B3%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%A7%D9%84%D8%A8%D8%B3%D8%A7%D8%B7%D9%8A</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/الجزائر</t>
+          <t>https://ar.wikipedia.org/wiki/مصر</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B5%D8%AE%D8%A8_%D8%A7%D9%84%D8%A8%D8%AD%D9%8A%D8%B1%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B3%D8%A7%D8%A6%D8%B1%D9%88%D9%86_%D9%86%D9%8A%D8%A7%D9%85%D8%A7_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%A7%D9%84%D8%A8%D8%B3%D8%A7%D8%B7%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B3%D8%B9%D8%AF_%D9%85%D9%83%D8%A7%D9%88%D9%8A</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2277,16 +2273,16 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%B3%D8%A7%D8%A6%D8%B1%D9%88%D9%86_%D9%86%D9%8A%D8%A7%D9%85%D8%A7_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/1952_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B3%D8%B9%D8%AF_%D9%85%D9%83%D8%A7%D9%88%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AC%D9%85%D9%8A%D9%84_%D8%B9%D8%B7%D9%8A%D8%A9_%D8%A5%D8%A8%D8%B1%D8%A7%D9%87%D9%8A%D9%85</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2297,281 +2293,241 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/1952_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%B7%D9%8A%D9%88%D8%B1_%D8%A3%D9%8A%D9%84%D9%88%D9%84_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AC%D9%85%D9%8A%D9%84_%D8%B9%D8%B7%D9%8A%D8%A9_%D8%A5%D8%A8%D8%B1%D8%A7%D9%87%D9%8A%D9%85</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A5%D9%85%D9%8A%D9%84%D9%8A_%D9%86%D8%B5%D8%B1_%D8%A7%D9%84%D9%84%D9%87</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/مصر</t>
+          <t>https://ar.wikipedia.org/wiki/لبنان</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%B7%D9%8A%D9%88%D8%B1_%D8%A3%D9%8A%D9%84%D9%88%D9%84_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A7%D9%84%D9%85%D8%A4%D8%A7%D9%85%D8%B1%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A5%D9%85%D9%8A%D9%84%D9%8A_%D9%86%D8%B5%D8%B1_%D8%A7%D9%84%D9%84%D9%87</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%81%D8%B1%D8%AC_%D8%A7%D9%84%D8%AD%D9%88%D8%A7%D8%B1</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/لبنان</t>
+          <t>https://ar.wikipedia.org/wiki/تونس</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A7%D9%84%D9%85%D8%A4%D8%A7%D9%85%D8%B1%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A7%D9%84%D9%85%D8%B9%D9%84%D9%85_%D8%B9%D9%84%D9%8A_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%81%D8%B1%D8%AC_%D8%A7%D9%84%D8%AD%D9%88%D8%A7%D8%B1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D9%83%D8%B1%D9%8A%D9%85_%D8%BA%D9%84%D8%A7%D8%A8</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/تونس</t>
+          <t>https://ar.wikipedia.org/wiki/المغرب</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A7%D9%84%D9%85%D8%B9%D9%84%D9%85_%D8%B9%D9%84%D9%8A_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%82%D8%A7%D9%85%D8%A7%D8%AA_%D8%A7%D9%84%D8%B2%D8%A8%D8%AF_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D9%83%D8%B1%D9%8A%D9%85_%D8%BA%D9%84%D8%A7%D8%A8</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A5%D9%84%D9%8A%D8%A7%D8%B3_%D9%81%D8%B1%D9%83%D9%88%D8%AD</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/المغرب</t>
+          <t>https://ar.wikipedia.org/wiki/الأردن</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%82%D8%A7%D9%85%D8%A7%D8%AA_%D8%A7%D9%84%D8%B2%D8%A8%D8%AF_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%B9%D8%B5%D8%A7%D9%81%D9%8A%D8%B1_%D8%A7%D9%84%D9%81%D8%AC%D8%B1_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A5%D9%84%D9%8A%D8%A7%D8%B3_%D9%81%D8%B1%D9%83%D9%88%D8%AD</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%84%D9%8A%D9%84%D9%89_%D8%B9%D8%B3%D9%8A%D8%B1%D8%A7%D9%86</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/الأردن</t>
+          <t>https://ar.wikipedia.org/wiki/لبنان</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%B9%D8%B5%D8%A7%D9%81%D9%8A%D8%B1_%D8%A7%D9%84%D9%81%D8%AC%D8%B1_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AC%D8%B3%D8%B1_%D8%A8%D9%86%D8%A7%D8%AA_%D9%8A%D8%B9%D9%82%D9%88%D8%A8_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%84%D9%8A%D9%84%D9%89_%D8%B9%D8%B3%D9%8A%D8%B1%D8%A7%D9%86</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%AD%D8%B3%D9%86_%D8%AD%D9%85%D9%8A%D8%AF</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/لبنان</t>
+          <t>https://ar.wikipedia.org/wiki/فلسطين</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AC%D8%B3%D8%B1_%D8%A8%D9%86%D8%A7%D8%AA_%D9%8A%D8%B9%D9%82%D9%88%D8%A8_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A7%D9%84%D9%88%D8%B3%D9%85%D9%8A%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%AD%D8%B3%D9%86_%D8%AD%D9%85%D9%8A%D8%AF</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D8%B9%D8%B2%D9%8A%D8%B2_%D9%85%D8%B4%D8%B1%D9%8A</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/فلسطين</t>
+          <t>https://ar.wikipedia.org/wiki/السعودية</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A7%D9%84%D9%88%D8%B3%D9%85%D9%8A%D8%A9_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A7%D9%84%D8%A8%D8%B4%D9%85%D9%88%D8%B1%D9%8A_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9_)&amp;action=edit&amp;redlink=1</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D8%B9%D8%B2%D9%8A%D8%B2_%D9%85%D8%B4%D8%B1%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B3%D9%84%D9%88%D9%89_%D8%A8%D9%83%D8%B1</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/السعودية</t>
+          <t>https://ar.wikipedia.org/wiki/مصر</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//w/index.php?title=%D8%A7%D9%84%D8%A8%D8%B4%D9%85%D9%88%D8%B1%D9%8A_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9_)&amp;action=edit&amp;redlink=1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%81%D8%A7%D8%B1%D8%B3_%D8%A7%D9%84%D9%82%D8%AA%D9%8A%D9%84_%D9%8A%D8%AA%D8%B1%D8%AC%D9%84_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B3%D9%84%D9%88%D9%89_%D8%A8%D9%83%D8%B1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A5%D9%84%D9%8A%D8%A7%D8%B3_%D8%A7%D9%84%D8%AF%D9%8A%D8%B1%D9%8A</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/مصر</t>
+          <t>https://ar.wikipedia.org/wiki/لبنان</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D9%81%D8%A7%D8%B1%D8%B3_%D8%A7%D9%84%D9%82%D8%AA%D9%8A%D9%84_%D9%8A%D8%AA%D8%B1%D8%AC%D9%84_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%AA%D9%88%D8%AA_%D8%A7%D9%84%D9%85%D8%B1</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A5%D9%84%D9%8A%D8%A7%D8%B3_%D8%A7%D9%84%D8%AF%D9%8A%D8%B1%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%A7%D9%84%D8%B9%D8%B1%D9%88%D8%B3%D9%8A_%D8%A7%D9%84%D9%85%D8%B7%D9%88%D9%8A</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/لبنان</t>
+          <t>https://ar.wikipedia.org/wiki/تونس</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%AA%D9%88%D8%AA_%D8%A7%D9%84%D9%85%D8%B1</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A3%D8%BA%D9%86%D9%8A%D8%A9_%D8%A7%D9%84%D9%85%D8%A7%D8%A1_%D9%88%D8%A7%D9%84%D9%86%D8%A7%D8%B1_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AD%D9%85%D8%AF_%D8%A7%D9%84%D8%B9%D8%B1%D9%88%D8%B3%D9%8A_%D8%A7%D9%84%D9%85%D8%B7%D9%88%D9%8A</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D9%84%D9%87_%D8%AE%D9%84%D9%8A%D9%81%D8%A9</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/تونس</t>
+          <t>https://ar.wikipedia.org/wiki/البحرين</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A3%D8%BA%D9%86%D9%8A%D8%A9_%D8%A7%D9%84%D9%85%D8%A7%D8%A1_%D9%88%D8%A7%D9%84%D9%86%D8%A7%D8%B1_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
+          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%A8%D8%A7%D8%A8_%D8%A7%D9%84%D9%85%D9%81%D8%AA%D9%88%D8%AD_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D9%84%D9%87_%D8%AE%D9%84%D9%8A%D9%81%D8%A9</t>
+          <t>https://ar.wikipedia.org//wiki/%D9%84%D8%B7%D9%8A%D9%81%D8%A9_%D8%A7%D9%84%D8%B2%D9%8A%D8%A7%D8%AA</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>https://ar.wikipedia.org/wiki/البحرين</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="n">
-        <v>105</v>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%A7%D9%84%D8%A8%D8%A7%D8%A8_%D8%A7%D9%84%D9%85%D9%81%D8%AA%D9%88%D8%AD_(%D8%B1%D9%88%D8%A7%D9%8A%D8%A9)</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%84%D8%B7%D9%8A%D9%81%D8%A9_%D8%A7%D9%84%D8%B2%D9%8A%D8%A7%D8%AA</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>https://ar.wikipedia.org/wiki/مصر</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="n">
-        <v>106</v>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>https://ar.wikipedia.org//wiki/%D9%85%D8%AF%D9%86_%D8%A7%D9%84%D9%85%D9%84%D8%AD</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>https://ar.wikipedia.org//wiki/%D8%B9%D8%A8%D8%AF_%D8%A7%D9%84%D8%B1%D8%AD%D9%85%D9%86_%D8%A7%D9%84%D9%85%D9%86%D9%8A%D9%81</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>https://ar.wikipedia.org/wiki/السعودية</t>
+          <t>https://ar.wikipedia.org/wiki/مصر</t>
         </is>
       </c>
     </row>

</xml_diff>